<commit_message>
fix: Fixed unclosed lines in scene 7.
</commit_message>
<xml_diff>
--- a/spreadsheets/formatted.xlsx
+++ b/spreadsheets/formatted.xlsx
@@ -29026,10 +29026,10 @@
     <t>しといてあげるね」</t>
   </si>
   <si>
-    <t>“Looks like I can rest here.</t>
-  </si>
-  <si>
-    <t>「ここで眠れるな……</t>
+    <t>“Looks like I can rest here.”</t>
+  </si>
+  <si>
+    <t>「ここで眠れるな……」</t>
   </si>
   <si>
     <t>Sleep</t>
@@ -29059,13 +29059,13 @@
     <t>TIFA,</t>
   </si>
   <si>
+    <t>ちゃ～んとAERITH助けてきてね」</t>
+  </si>
+  <si>
     <t>CLOUD!</t>
   </si>
   <si>
     <t>Please bring AERIS back!”</t>
-  </si>
-  <si>
-    <t>ちゃ～んとAERITH助けてきてね」}</t>
   </si>
   <si>
     <t>“You're going after AERIS, right?”</t>
@@ -83543,19 +83543,18 @@
       <c r="A229" s="29" t="s">
         <v>9664</v>
       </c>
-      <c r="B229" s="2"/>
+      <c r="B229" s="30" t="s">
+        <v>9665</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="29" t="s">
-        <v>9665</v>
+        <v>9666</v>
       </c>
       <c r="B230" s="2"/>
     </row>
     <row r="231">
       <c r="A231" s="29" t="s">
-        <v>9666</v>
-      </c>
-      <c r="B231" s="30" t="s">
         <v>9667</v>
       </c>
     </row>

</xml_diff>